<commit_message>
ranking was trouble shooted
</commit_message>
<xml_diff>
--- a/7_Part 4 Graphics/Stadtteile_Ranking.xlsx
+++ b/7_Part 4 Graphics/Stadtteile_Ranking.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Sheet1'!$A$1:$C$28</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Sheet1'!$A$1:$D$28</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -433,7 +433,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -443,13 +443,14 @@
   <cols>
     <col width="24" customWidth="1" min="1" max="1"/>
     <col width="15" customWidth="1" min="2" max="2"/>
-    <col width="14" customWidth="1" min="3" max="3"/>
+    <col width="24" customWidth="1" min="3" max="3"/>
+    <col width="14" customWidth="1" min="4" max="4"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="inlineStr">
         <is>
-          <t>Stadtteil</t>
+          <t>Start Stadtteil</t>
         </is>
       </c>
       <c r="B1" s="2" t="inlineStr">
@@ -458,6 +459,11 @@
         </is>
       </c>
       <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>Ziel Stadtteil</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
         <is>
           <t>Anzahl Ziele</t>
         </is>
@@ -472,7 +478,12 @@
       <c r="B2" s="3" t="n">
         <v>2258</v>
       </c>
-      <c r="C2" s="3" t="n">
+      <c r="C2" s="3" t="inlineStr">
+        <is>
+          <t>Innenstadt-West</t>
+        </is>
+      </c>
+      <c r="D2" s="3" t="n">
         <v>2258</v>
       </c>
     </row>
@@ -485,7 +496,12 @@
       <c r="B3" s="3" t="n">
         <v>534</v>
       </c>
-      <c r="C3" s="3" t="n">
+      <c r="C3" s="3" t="inlineStr">
+        <is>
+          <t>Hagsfeld</t>
+        </is>
+      </c>
+      <c r="D3" s="3" t="n">
         <v>534</v>
       </c>
     </row>
@@ -498,7 +514,12 @@
       <c r="B4" s="3" t="n">
         <v>473</v>
       </c>
-      <c r="C4" s="3" t="n">
+      <c r="C4" s="3" t="inlineStr">
+        <is>
+          <t>Oststadt</t>
+        </is>
+      </c>
+      <c r="D4" s="3" t="n">
         <v>473</v>
       </c>
     </row>
@@ -511,7 +532,12 @@
       <c r="B5" s="3" t="n">
         <v>340</v>
       </c>
-      <c r="C5" s="3" t="n">
+      <c r="C5" s="3" t="inlineStr">
+        <is>
+          <t>Stupferich</t>
+        </is>
+      </c>
+      <c r="D5" s="3" t="n">
         <v>340</v>
       </c>
     </row>
@@ -524,7 +550,12 @@
       <c r="B6" s="3" t="n">
         <v>261</v>
       </c>
-      <c r="C6" s="3" t="n">
+      <c r="C6" s="3" t="inlineStr">
+        <is>
+          <t>Südweststadt</t>
+        </is>
+      </c>
+      <c r="D6" s="3" t="n">
         <v>261</v>
       </c>
     </row>
@@ -537,7 +568,12 @@
       <c r="B7" s="3" t="n">
         <v>231</v>
       </c>
-      <c r="C7" s="3" t="n">
+      <c r="C7" s="3" t="inlineStr">
+        <is>
+          <t>Durlach</t>
+        </is>
+      </c>
+      <c r="D7" s="3" t="n">
         <v>231</v>
       </c>
     </row>
@@ -550,7 +586,12 @@
       <c r="B8" s="3" t="n">
         <v>224</v>
       </c>
-      <c r="C8" s="3" t="n">
+      <c r="C8" s="3" t="inlineStr">
+        <is>
+          <t>Grötzingen</t>
+        </is>
+      </c>
+      <c r="D8" s="3" t="n">
         <v>224</v>
       </c>
     </row>
@@ -563,7 +604,12 @@
       <c r="B9" s="3" t="n">
         <v>216</v>
       </c>
-      <c r="C9" s="3" t="n">
+      <c r="C9" s="3" t="inlineStr">
+        <is>
+          <t>Weststadt</t>
+        </is>
+      </c>
+      <c r="D9" s="3" t="n">
         <v>216</v>
       </c>
     </row>
@@ -576,7 +622,12 @@
       <c r="B10" s="3" t="n">
         <v>162</v>
       </c>
-      <c r="C10" s="3" t="n">
+      <c r="C10" s="3" t="inlineStr">
+        <is>
+          <t>Südstadt</t>
+        </is>
+      </c>
+      <c r="D10" s="3" t="n">
         <v>162</v>
       </c>
     </row>
@@ -589,7 +640,12 @@
       <c r="B11" s="3" t="n">
         <v>159</v>
       </c>
-      <c r="C11" s="3" t="n">
+      <c r="C11" s="3" t="inlineStr">
+        <is>
+          <t>Neureut</t>
+        </is>
+      </c>
+      <c r="D11" s="3" t="n">
         <v>159</v>
       </c>
     </row>
@@ -602,7 +658,12 @@
       <c r="B12" s="3" t="n">
         <v>136</v>
       </c>
-      <c r="C12" s="3" t="n">
+      <c r="C12" s="3" t="inlineStr">
+        <is>
+          <t>Mühlburg</t>
+        </is>
+      </c>
+      <c r="D12" s="3" t="n">
         <v>136</v>
       </c>
     </row>
@@ -615,7 +676,12 @@
       <c r="B13" s="3" t="n">
         <v>113</v>
       </c>
-      <c r="C13" s="3" t="n">
+      <c r="C13" s="3" t="inlineStr">
+        <is>
+          <t>Rintheim</t>
+        </is>
+      </c>
+      <c r="D13" s="3" t="n">
         <v>113</v>
       </c>
     </row>
@@ -628,7 +694,12 @@
       <c r="B14" s="3" t="n">
         <v>110</v>
       </c>
-      <c r="C14" s="3" t="n">
+      <c r="C14" s="3" t="inlineStr">
+        <is>
+          <t>Nordstadt</t>
+        </is>
+      </c>
+      <c r="D14" s="3" t="n">
         <v>110</v>
       </c>
     </row>
@@ -641,7 +712,12 @@
       <c r="B15" s="3" t="n">
         <v>99</v>
       </c>
-      <c r="C15" s="3" t="n">
+      <c r="C15" s="3" t="inlineStr">
+        <is>
+          <t>Weiherfeld-Dammerstock</t>
+        </is>
+      </c>
+      <c r="D15" s="3" t="n">
         <v>99</v>
       </c>
     </row>
@@ -654,7 +730,12 @@
       <c r="B16" s="3" t="n">
         <v>95</v>
       </c>
-      <c r="C16" s="3" t="n">
+      <c r="C16" s="3" t="inlineStr">
+        <is>
+          <t>Palmbach</t>
+        </is>
+      </c>
+      <c r="D16" s="3" t="n">
         <v>95</v>
       </c>
     </row>
@@ -667,7 +748,12 @@
       <c r="B17" s="3" t="n">
         <v>65</v>
       </c>
-      <c r="C17" s="3" t="n">
+      <c r="C17" s="3" t="inlineStr">
+        <is>
+          <t>Grünwettersbach</t>
+        </is>
+      </c>
+      <c r="D17" s="3" t="n">
         <v>65</v>
       </c>
     </row>
@@ -680,7 +766,12 @@
       <c r="B18" s="3" t="n">
         <v>60</v>
       </c>
-      <c r="C18" s="3" t="n">
+      <c r="C18" s="3" t="inlineStr">
+        <is>
+          <t>Rüppurr</t>
+        </is>
+      </c>
+      <c r="D18" s="3" t="n">
         <v>60</v>
       </c>
     </row>
@@ -693,7 +784,12 @@
       <c r="B19" s="3" t="n">
         <v>59</v>
       </c>
-      <c r="C19" s="3" t="n">
+      <c r="C19" s="3" t="inlineStr">
+        <is>
+          <t>Nordweststadt</t>
+        </is>
+      </c>
+      <c r="D19" s="3" t="n">
         <v>59</v>
       </c>
     </row>
@@ -706,7 +802,12 @@
       <c r="B20" s="3" t="n">
         <v>58</v>
       </c>
-      <c r="C20" s="3" t="n">
+      <c r="C20" s="3" t="inlineStr">
+        <is>
+          <t>Waldstadt</t>
+        </is>
+      </c>
+      <c r="D20" s="3" t="n">
         <v>58</v>
       </c>
     </row>
@@ -719,7 +820,12 @@
       <c r="B21" s="3" t="n">
         <v>57</v>
       </c>
-      <c r="C21" s="3" t="n">
+      <c r="C21" s="3" t="inlineStr">
+        <is>
+          <t>Daxlanden</t>
+        </is>
+      </c>
+      <c r="D21" s="3" t="n">
         <v>57</v>
       </c>
     </row>
@@ -732,7 +838,12 @@
       <c r="B22" s="3" t="n">
         <v>55</v>
       </c>
-      <c r="C22" s="3" t="n">
+      <c r="C22" s="3" t="inlineStr">
+        <is>
+          <t>Knielingen</t>
+        </is>
+      </c>
+      <c r="D22" s="3" t="n">
         <v>55</v>
       </c>
     </row>
@@ -745,7 +856,12 @@
       <c r="B23" s="3" t="n">
         <v>54</v>
       </c>
-      <c r="C23" s="3" t="n">
+      <c r="C23" s="3" t="inlineStr">
+        <is>
+          <t>Oberreut</t>
+        </is>
+      </c>
+      <c r="D23" s="3" t="n">
         <v>54</v>
       </c>
     </row>
@@ -758,7 +874,12 @@
       <c r="B24" s="3" t="n">
         <v>53</v>
       </c>
-      <c r="C24" s="3" t="n">
+      <c r="C24" s="3" t="inlineStr">
+        <is>
+          <t>Innenstadt-Ost</t>
+        </is>
+      </c>
+      <c r="D24" s="3" t="n">
         <v>53</v>
       </c>
     </row>
@@ -771,7 +892,12 @@
       <c r="B25" s="3" t="n">
         <v>51</v>
       </c>
-      <c r="C25" s="3" t="n">
+      <c r="C25" s="3" t="inlineStr">
+        <is>
+          <t>Hohenwettersbach</t>
+        </is>
+      </c>
+      <c r="D25" s="3" t="n">
         <v>51</v>
       </c>
     </row>
@@ -784,7 +910,12 @@
       <c r="B26" s="3" t="n">
         <v>50</v>
       </c>
-      <c r="C26" s="3" t="n">
+      <c r="C26" s="3" t="inlineStr">
+        <is>
+          <t>Wolfartsweier</t>
+        </is>
+      </c>
+      <c r="D26" s="3" t="n">
         <v>50</v>
       </c>
     </row>
@@ -797,7 +928,12 @@
       <c r="B27" s="3" t="n">
         <v>40</v>
       </c>
-      <c r="C27" s="3" t="n">
+      <c r="C27" s="3" t="inlineStr">
+        <is>
+          <t>Beiertheim-Bulach</t>
+        </is>
+      </c>
+      <c r="D27" s="3" t="n">
         <v>40</v>
       </c>
     </row>
@@ -810,12 +946,17 @@
       <c r="B28" s="3" t="n">
         <v>40</v>
       </c>
-      <c r="C28" s="3" t="n">
+      <c r="C28" s="3" t="inlineStr">
+        <is>
+          <t>Grünwinkel</t>
+        </is>
+      </c>
+      <c r="D28" s="3" t="n">
         <v>40</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C28"/>
+  <autoFilter ref="A1:D28"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>